<commit_message>
Update readme, templates and add oech_rpm_version_designn
</commit_message>
<xml_diff>
--- a/templates/板卡兼容性发布清单模板.xlsx
+++ b/templates/板卡兼容性发布清单模板.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20387"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Station\Gitee\oec-hardware\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07AE910-AEB3-482D-B2B3-AF46E9A48FA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA34A01-E2DB-459F-AD05-7C35E3A492A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9880" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>vendorID</t>
   </si>
@@ -65,102 +65,131 @@
     <t>string</t>
   </si>
   <si>
-    <t>Intel XL710QSR1G1P5</t>
-  </si>
-  <si>
-    <t>FAIL 速率不达标</t>
-  </si>
-  <si>
-    <t>MCX516A-CCAT</t>
-  </si>
-  <si>
-    <t>板卡</t>
-  </si>
-  <si>
-    <t>问题</t>
-  </si>
-  <si>
     <t>date</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>chipVendor</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>boardModel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>chipModel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>downloadLink</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>架构</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>操作系统版本</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>驱动名称</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>驱动版本</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>板卡类型</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>认证日期</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>驱动的sha256</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>驱动大小</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>芯片厂商</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>板卡型号</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>芯片型号</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编码(选填）</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>驱动下载链接</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>板卡四元组</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>板卡四元组查看方式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 使用 lspci -nvv 查看</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 使用 lspci -xs 查看</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取方式：lspci -nvv</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uname -m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>grep openeulerversion /etc/openEuler-latest</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sha256sum $(modinfo driver_name | grep filename | awk '{print $2}')</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modinfo driver_name | grep version</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ll $(modinfo driver_name | grep filename | awk '{print $2}') | awk '{print $5}'</t>
+  </si>
+  <si>
+    <t>内核驱动写：inbox
+外部驱动写下载链接</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可从iBMC上获取</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,21 +199,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -205,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,12 +241,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +315,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -342,29 +350,51 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -383,6 +413,129 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>26411</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD990962-12FC-4256-A2E7-94F9D0521245}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95251" y="558800"/>
+          <a:ext cx="7506710" cy="1695450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6830C2F-6C46-4CA7-9267-011B45B3F906}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3041650"/>
+          <a:ext cx="5270500" cy="2063750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -672,11 +825,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -691,13 +844,13 @@
     <col min="8" max="8" width="24.90625" style="6" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" customWidth="1"/>
     <col min="10" max="10" width="13.08984375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="56.26953125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="16.6328125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="47.1796875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="33.54296875" style="6" customWidth="1"/>
     <col min="13" max="13" width="16.08984375" style="6" customWidth="1"/>
     <col min="14" max="14" width="32.7265625" style="6" customWidth="1"/>
     <col min="15" max="15" width="17.7265625" style="6" customWidth="1"/>
     <col min="16" max="16" width="22.26953125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="13.81640625" style="6" customWidth="1"/>
+    <col min="17" max="17" width="19.90625" style="6" customWidth="1"/>
     <col min="18" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -729,8 +882,8 @@
       <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="18" t="s">
-        <v>18</v>
+      <c r="J1" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>9</v>
@@ -738,20 +891,20 @@
       <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>21</v>
+      <c r="M1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="18" t="s">
-        <v>22</v>
+      <c r="Q1" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -808,59 +961,93 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>35</v>
+      <c r="F4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="27"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="19" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" insertHyperlinks="0" autoFilter="0"/>
   <autoFilter ref="A1:Q3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="M4:O4"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
@@ -868,81 +1055,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="18.453125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2"/>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2"/>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>14</v>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" insertHyperlinks="0" autoFilter="0"/>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;F&amp;R文档密级</oddHeader>
     <oddFooter>&amp;L&amp;D&amp;C华为保密信息,未经授权禁止扩散&amp;R第&amp;P页，共&amp;N页</oddFooter>
   </headerFooter>
-  <legacyDrawingHF r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawingHF r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <pixelatorList sheetStid="1"/>
-  <pixelatorList sheetStid="2"/>
-  <pixelatorList sheetStid="3"/>
-  <pixelatorList sheetStid="4"/>
-</pixelators>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <allowEditUser xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" hasInvisiblePropRange="0">
   <rangeList sheetStid="1" master=""/>
   <rangeList sheetStid="2" master=""/>
@@ -950,7 +1104,7 @@
 </allowEditUser>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <woProps xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <woSheetsProps>
     <woSheetProps sheetStid="1" interlineOnOff="0" interlineColor="0" isDbSheet="0" isDashBoardSheet="0"/>
@@ -963,7 +1117,38 @@
 </woProps>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <pixelatorList sheetStid="1"/>
+  <pixelatorList sheetStid="2"/>
+  <pixelatorList sheetStid="3"/>
+  <pixelatorList sheetStid="4"/>
+</pixelators>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5607D9-04D2-4DE1-AC0E-A7772F01BC71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06A0048C-2381-489B-AA07-9611017176EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
@@ -972,29 +1157,11 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5607D9-04D2-4DE1-AC0E-A7772F01BC71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>